<commit_message>
tokyo nova typo fix
</commit_message>
<xml_diff>
--- a/tokyo-nova/checklist.xlsx
+++ b/tokyo-nova/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/tokyo-nova/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B566D9A-F2AC-984B-9F00-327E8324F33C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC5B973-0AB7-E043-B54D-CBF238805CA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{22EAF693-7861-A34E-A783-34EF7D154F64}"/>
   </bookViews>
@@ -119,9 +119,6 @@
     <t>猟犬たちの午後―トーキョーNOVA The 2nd Editionリプレイ</t>
   </si>
   <si>
-    <t>Hounds Afternoon: Toky Nova The 2nd Edition Replay</t>
-  </si>
-  <si>
     <t>tokyo_nova_replay_2nd_ed.jpg</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>scenario</t>
+  </si>
+  <si>
+    <t>Hounds Afternoon: Tokyo Nova The 2nd Edition Replay</t>
   </si>
 </sst>
 </file>
@@ -501,7 +501,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,7 +529,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -549,7 +549,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -569,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -589,7 +589,7 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -600,16 +600,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -629,7 +629,7 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -649,7 +649,7 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -669,7 +669,7 @@
         <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tokyo nova 2nd ed handbook
</commit_message>
<xml_diff>
--- a/tokyo-nova/checklist.xlsx
+++ b/tokyo-nova/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/tokyo-nova/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0671C62E-36B2-5046-9C49-D51C9EE93E76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284B90FA-ECC4-E640-B8DD-F5BAF35CDDB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{22EAF693-7861-A34E-A783-34EF7D154F64}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>Hounds Afternoon: Tokyo Nova The 2nd Edition Replay</t>
+  </si>
+  <si>
+    <t>tokyo_nova_handbook.jpg</t>
+  </si>
+  <si>
+    <t>トーキョーN◎VA The 2nd Edition ハンドブック</t>
+  </si>
+  <si>
+    <t>Tokyo Nova: The 2nd Edition: Handbook</t>
   </si>
 </sst>
 </file>
@@ -498,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4679E55C-30BE-044D-B3AF-8434FCFD3724}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,16 +626,16 @@
         <v>1996</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
         <v>32</v>
@@ -634,19 +643,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
         <v>32</v>
@@ -657,18 +666,38 @@
         <v>1997</v>
       </c>
       <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1997</v>
+      </c>
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>24</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more tokyo nova images
</commit_message>
<xml_diff>
--- a/tokyo-nova/checklist.xlsx
+++ b/tokyo-nova/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/tokyo-nova/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB07AD3A-E1EC-484B-ADFB-EEA8C993400E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB1D9E1-A3C4-8448-ACCD-2BDC272D7EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{22EAF693-7861-A34E-A783-34EF7D154F64}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="162">
   <si>
     <t>year</t>
   </si>
@@ -449,37 +449,76 @@
     <t>counterglow_replay.jpg</t>
   </si>
   <si>
-    <t>トーキョーN◎VA The Detonation スーパー・シナリオ・サポート Vol. 1</t>
-  </si>
-  <si>
-    <t>トーキョーN◎VA The Detonation スーパー・シナリオ・サポート Vol. 2</t>
-  </si>
-  <si>
-    <t>トーキョーN◎VA The Detonation スーパー・シナリオ・サポート Vol. 3</t>
-  </si>
-  <si>
-    <t>トーキョーN◎VA The Detonation スーパー・シナリオ・サポート Vol. 4</t>
-  </si>
-  <si>
-    <t>トーキョーN◎VA The Detonation スーパー・シナリオ・サポート Vol. 5</t>
-  </si>
-  <si>
     <t>sssdet4.jpg</t>
   </si>
   <si>
-    <t>Tokyo Nova The Detonation Super Scenario Support Vol. 1</t>
-  </si>
-  <si>
-    <t>Tokyo Nova The Detonation Super Scenario Support Vol. 2</t>
-  </si>
-  <si>
-    <t>Tokyo Nova The Detonation Super Scenario Support Vol. 3</t>
-  </si>
-  <si>
-    <t>Tokyo Nova The Detonation Super Scenario Support Vol. 4</t>
-  </si>
-  <si>
-    <t>Tokyo Nova The Detonation Super Scenario Support Vol. 5</t>
+    <t>Tokyo Nova The Detonation Super Scenario Support Vol. 2: World of Darkness</t>
+  </si>
+  <si>
+    <t>トーキョーN◎VA The Detonation スーパー・シナリオ・サポート Vol. 2 暗黒の世界</t>
+  </si>
+  <si>
+    <t>sssdet2.jpg</t>
+  </si>
+  <si>
+    <t>トーキョーN◎VA The Detonation スーパー・シナリオ・サポート Vol. 3 仮面舞踏会</t>
+  </si>
+  <si>
+    <t>Tokyo Nova The Detonation Super Scenario Support Vol. 3: Behind the Mask</t>
+  </si>
+  <si>
+    <t>sssdet3.jpg</t>
+  </si>
+  <si>
+    <t>Tokyo Nova The Detonation Super Scenario Support Vol. 1: Crystal Wall</t>
+  </si>
+  <si>
+    <t>sssdet1.jpg</t>
+  </si>
+  <si>
+    <t>sssdet1a.jpg</t>
+  </si>
+  <si>
+    <t>トーキョーN◎VA The Detonation スーパー・シナリオ・サポート Vol. 1 フロントライン</t>
+  </si>
+  <si>
+    <t>sssdet2a.jpg</t>
+  </si>
+  <si>
+    <t>トーキョーN◎VA The Detonation スーパー・シナリオ・サポート Vol. 3 フロントライン</t>
+  </si>
+  <si>
+    <t>トーキョーN◎VA The Detonation スーパー・シナリオ・サポート Vol. 1 この声がとどくまで</t>
+  </si>
+  <si>
+    <t>Tokyo Nova The Detonation Super Scenario Support Vol. 3: Calling You</t>
+  </si>
+  <si>
+    <t>sssdet3a.jpg</t>
+  </si>
+  <si>
+    <t>Tokyo Nova The Detonation Super Scenario Support Vol. 2: Flaming Fish</t>
+  </si>
+  <si>
+    <t>トーキョーN◎VA The Detonation スーパー・シナリオ・サポート Vol. 2 魂こがして</t>
+  </si>
+  <si>
+    <t>Tokyo Nova The Detonation Super Scenario Support Vol. 1: Froneline</t>
+  </si>
+  <si>
+    <t>トーキョーN◎VA The Detonation スーパー・シナリオ・サポート Vol. 4 人間以上</t>
+  </si>
+  <si>
+    <t>Tokyo Nova The Detonation Super Scenario Support Vol. 4: Manplus</t>
+  </si>
+  <si>
+    <t>トーキョーN◎VA The Detonation スーパー・シナリオ・サポート Vol. 5 夕日の沈む朝</t>
+  </si>
+  <si>
+    <t>Tokyo Nova The Detonation Super Scenario Support Vol. 5: The Sun Against the Sun</t>
+  </si>
+  <si>
+    <t>sssdet5.jpg</t>
   </si>
 </sst>
 </file>
@@ -856,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4679E55C-30BE-044D-B3AF-8434FCFD3724}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44:D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1698,60 +1737,162 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2003</v>
+      </c>
       <c r="B44" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" t="s">
+        <v>147</v>
+      </c>
+      <c r="F44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2004</v>
+      </c>
+      <c r="B45" t="s">
+        <v>155</v>
+      </c>
+      <c r="C45" t="s">
+        <v>154</v>
+      </c>
+      <c r="D45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" t="s">
+        <v>149</v>
+      </c>
+      <c r="F45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2004</v>
+      </c>
+      <c r="B46" t="s">
+        <v>150</v>
+      </c>
+      <c r="C46" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" t="s">
+        <v>153</v>
+      </c>
+      <c r="F46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2005</v>
+      </c>
+      <c r="B47" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" t="s">
+        <v>145</v>
+      </c>
+      <c r="D47" t="s">
+        <v>23</v>
+      </c>
+      <c r="E47" t="s">
+        <v>146</v>
+      </c>
+      <c r="F47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2005</v>
+      </c>
+      <c r="B48" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" t="s">
+        <v>141</v>
+      </c>
+      <c r="F48" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2005</v>
+      </c>
+      <c r="B49" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" t="s">
+        <v>143</v>
+      </c>
+      <c r="D49" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" t="s">
+        <v>144</v>
+      </c>
+      <c r="F49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2005</v>
+      </c>
+      <c r="B50" t="s">
+        <v>157</v>
+      </c>
+      <c r="C50" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" t="s">
         <v>138</v>
       </c>
-      <c r="C44" t="s">
-        <v>144</v>
-      </c>
-      <c r="F44" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>139</v>
-      </c>
-      <c r="C45" t="s">
-        <v>145</v>
-      </c>
-      <c r="F45" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>140</v>
-      </c>
-      <c r="C46" t="s">
-        <v>146</v>
-      </c>
-      <c r="F46" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
-        <v>141</v>
-      </c>
-      <c r="C47" t="s">
-        <v>147</v>
-      </c>
-      <c r="E47" t="s">
-        <v>143</v>
-      </c>
-      <c r="F47" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>142</v>
-      </c>
-      <c r="C48" t="s">
-        <v>148</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="F50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2004</v>
+      </c>
+      <c r="B51" t="s">
+        <v>159</v>
+      </c>
+      <c r="C51" t="s">
+        <v>160</v>
+      </c>
+      <c r="D51" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" t="s">
+        <v>161</v>
+      </c>
+      <c r="F51" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>